<commit_message>
post topics for the new school year
</commit_message>
<xml_diff>
--- a/topics/2023.Fall.Assignment Subjects_SWR302_SWP391_FER201M_SWT_PRN.xlsx
+++ b/topics/2023.Fall.Assignment Subjects_SWR302_SWP391_FER201M_SWT_PRN.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26831"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{38464281-63FB-4840-9E33-6510EE108FF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{56E21A0F-53E7-43C0-BC15-9DAD603B94B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="4" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="482" uniqueCount="316">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="321">
   <si>
     <t>No</t>
   </si>
@@ -1660,6 +1660,44 @@
 hình ảnh, bao gồm logo dựa trên mẫu được định nghĩa trước do admin.</t>
   </si>
   <si>
+    <t>Zoo Management Application</t>
+  </si>
+  <si>
+    <t>Quản lý thông tin trong Zoo hiện tại thực hiện bằng tay, nhu cầu số hóa hệ thống và thống kê dữ liệu là cấp bách.</t>
+  </si>
+  <si>
+    <t>Quản lý vé vào cổng của Zoo, thống kê dữ liệu theo ngày, tuần, tháng, năm
+Quản lý thông tin liên quan đến Animal, Animal species
+Quản lý tin tức của Zoo
+Quản lý khu vực trong sở thú (1 sở thú có nhiều khu vực A, B, C). Trong 1 khu vực sẽ có nhiều chuồng thú, mỗi chuồng thú sẽ được ghi nhận với mã số chuồng AXXXX. 
+Khi 1 con Animal được chuyển về Zoo, nó sẽ được tạo 1 hồ sơ và đưa vào 1 chuồng thú (animal cage) và được gán với 1 người huấn luyện thú (animal trainer). Người huấn luyện thú này có nhiệm vụ cập nhật các thông tin liên quan đến  Animal.
+Quản lý đồ ăn hàng ngày cho các con Animal trong Zoo. Mỗi con Animal sẽ có 1 chế độ ăn khác nhau.</t>
+  </si>
+  <si>
+    <t>Guest -  người tham quan Zoo
+Staff 
+Zoo Trainer
+Administrator</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Guest 
+- Mua vé tham gia zoo trực tuyến 
+Staff
+- Quản lý thông tin khu vực
+- Quản lý thông tin chuồng thú
+- Manage Zoo Trainer account
+- Quản lý tin tức của Zoo
+- Thống kê dữ liệu
+Zoo Trainer
+- Quản lý thông tin Animal, Animal species
+- Quản lý/theo dõi việc ăn uống của các Animal 
+- Quản lý kinh nghiệm cá nhân
+Admin
+- Quản lý Staff account
+- Quản lý cấu hình hệ thống
+</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="11"/>
@@ -1848,9 +1886,8 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-      <charset val="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="6">
@@ -1885,7 +1922,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="23">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -2196,22 +2233,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="111">
+  <cellXfs count="96">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment readingOrder="1"/>
@@ -2404,20 +2430,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -2431,83 +2448,8 @@
     <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="18" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="21" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -2527,17 +2469,56 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="23" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -65071,8 +65052,8 @@
   <dimension ref="A1:AB39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D32" sqref="D32"/>
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G30" sqref="A2:G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -65086,25 +65067,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" s="59" customFormat="1" ht="27" customHeight="1">
-      <c r="A1" s="70" t="s">
+      <c r="A1" s="94" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="69" t="s">
+      <c r="B1" s="95" t="s">
         <v>190</v>
       </c>
-      <c r="C1" s="69" t="s">
+      <c r="C1" s="95" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="69" t="s">
+      <c r="D1" s="95" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="69" t="s">
+      <c r="E1" s="95" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="69" t="s">
+      <c r="F1" s="95" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="69" t="s">
+      <c r="G1" s="95" t="s">
         <v>7</v>
       </c>
       <c r="H1" s="60"/>
@@ -65133,22 +65114,22 @@
       <c r="A2" s="85">
         <v>1</v>
       </c>
-      <c r="B2" s="103" t="s">
+      <c r="B2" s="75" t="s">
         <v>219</v>
       </c>
-      <c r="C2" s="103" t="s">
+      <c r="C2" s="75" t="s">
         <v>220</v>
       </c>
-      <c r="D2" s="103" t="s">
+      <c r="D2" s="75" t="s">
         <v>221</v>
       </c>
-      <c r="E2" s="103" t="s">
+      <c r="E2" s="75" t="s">
         <v>222</v>
       </c>
-      <c r="F2" s="103" t="s">
+      <c r="F2" s="75" t="s">
         <v>223</v>
       </c>
-      <c r="G2" s="103"/>
+      <c r="G2" s="75"/>
       <c r="H2" s="62"/>
       <c r="I2" s="63"/>
       <c r="J2" s="64"/>
@@ -65172,485 +65153,497 @@
       <c r="AB2" s="65"/>
     </row>
     <row r="3" spans="1:28" s="55" customFormat="1" ht="48" customHeight="1">
-      <c r="A3" s="86"/>
-      <c r="B3" s="103"/>
-      <c r="C3" s="103"/>
-      <c r="D3" s="103"/>
-      <c r="E3" s="103" t="s">
+      <c r="A3" s="85"/>
+      <c r="B3" s="75"/>
+      <c r="C3" s="75"/>
+      <c r="D3" s="75"/>
+      <c r="E3" s="75" t="s">
         <v>224</v>
       </c>
-      <c r="F3" s="103" t="s">
+      <c r="F3" s="75" t="s">
         <v>225</v>
       </c>
-      <c r="G3" s="104"/>
+      <c r="G3" s="76"/>
       <c r="H3" s="62"/>
       <c r="I3" s="63"/>
     </row>
-    <row r="4" spans="1:28" s="55" customFormat="1" ht="45.75">
-      <c r="A4" s="86"/>
-      <c r="B4" s="103"/>
-      <c r="C4" s="103"/>
-      <c r="D4" s="103"/>
-      <c r="E4" s="103" t="s">
+    <row r="4" spans="1:28" s="55" customFormat="1">
+      <c r="A4" s="85"/>
+      <c r="B4" s="75"/>
+      <c r="C4" s="75"/>
+      <c r="D4" s="75"/>
+      <c r="E4" s="75" t="s">
         <v>226</v>
       </c>
-      <c r="F4" s="103" t="s">
+      <c r="F4" s="75" t="s">
         <v>227</v>
       </c>
-      <c r="G4" s="104"/>
+      <c r="G4" s="76"/>
       <c r="H4" s="62"/>
       <c r="I4" s="63"/>
     </row>
-    <row r="5" spans="1:28" s="55" customFormat="1" ht="30.75">
-      <c r="A5" s="87"/>
-      <c r="B5" s="103"/>
-      <c r="C5" s="103"/>
-      <c r="D5" s="103"/>
-      <c r="E5" s="103" t="s">
+    <row r="5" spans="1:28" s="55" customFormat="1">
+      <c r="A5" s="85"/>
+      <c r="B5" s="75"/>
+      <c r="C5" s="75"/>
+      <c r="D5" s="75"/>
+      <c r="E5" s="75" t="s">
         <v>217</v>
       </c>
-      <c r="F5" s="103" t="s">
+      <c r="F5" s="75" t="s">
         <v>228</v>
       </c>
-      <c r="G5" s="104"/>
+      <c r="G5" s="76"/>
       <c r="H5" s="62"/>
       <c r="I5" s="63"/>
     </row>
     <row r="6" spans="1:28" s="55" customFormat="1" ht="213">
-      <c r="A6" s="88">
+      <c r="A6" s="86">
         <v>2</v>
       </c>
-      <c r="B6" s="105" t="s">
+      <c r="B6" s="77" t="s">
         <v>239</v>
       </c>
-      <c r="C6" s="105" t="s">
+      <c r="C6" s="77" t="s">
         <v>240</v>
       </c>
-      <c r="D6" s="105" t="s">
+      <c r="D6" s="77" t="s">
         <v>241</v>
       </c>
-      <c r="E6" s="105" t="s">
+      <c r="E6" s="77" t="s">
         <v>197</v>
       </c>
-      <c r="F6" s="105" t="s">
+      <c r="F6" s="77" t="s">
         <v>242</v>
       </c>
-      <c r="G6" s="105"/>
-    </row>
-    <row r="7" spans="1:28" s="55" customFormat="1" ht="30.75">
-      <c r="A7" s="89"/>
-      <c r="B7" s="105"/>
-      <c r="C7" s="105"/>
-      <c r="D7" s="105"/>
-      <c r="E7" s="105" t="s">
+      <c r="G6" s="77"/>
+    </row>
+    <row r="7" spans="1:28" s="55" customFormat="1">
+      <c r="A7" s="86"/>
+      <c r="B7" s="77"/>
+      <c r="C7" s="77"/>
+      <c r="D7" s="77"/>
+      <c r="E7" s="77" t="s">
         <v>243</v>
       </c>
-      <c r="F7" s="105" t="s">
+      <c r="F7" s="77" t="s">
         <v>244</v>
       </c>
-      <c r="G7" s="105"/>
+      <c r="G7" s="77"/>
     </row>
     <row r="8" spans="1:28" s="55" customFormat="1">
-      <c r="A8" s="89"/>
-      <c r="B8" s="105"/>
-      <c r="C8" s="105"/>
-      <c r="D8" s="105"/>
-      <c r="E8" s="105" t="s">
+      <c r="A8" s="86"/>
+      <c r="B8" s="77"/>
+      <c r="C8" s="77"/>
+      <c r="D8" s="77"/>
+      <c r="E8" s="77" t="s">
         <v>195</v>
       </c>
-      <c r="F8" s="105" t="s">
+      <c r="F8" s="77" t="s">
         <v>245</v>
       </c>
-      <c r="G8" s="105"/>
-    </row>
-    <row r="9" spans="1:28" s="55" customFormat="1" ht="30.75">
-      <c r="A9" s="90"/>
-      <c r="B9" s="105"/>
-      <c r="C9" s="105"/>
-      <c r="D9" s="105"/>
-      <c r="E9" s="105" t="s">
+      <c r="G8" s="77"/>
+    </row>
+    <row r="9" spans="1:28" s="55" customFormat="1">
+      <c r="A9" s="86"/>
+      <c r="B9" s="77"/>
+      <c r="C9" s="77"/>
+      <c r="D9" s="77"/>
+      <c r="E9" s="77" t="s">
         <v>217</v>
       </c>
-      <c r="F9" s="105" t="s">
+      <c r="F9" s="77" t="s">
         <v>246</v>
       </c>
-      <c r="G9" s="105"/>
-    </row>
-    <row r="10" spans="1:28" s="68" customFormat="1" ht="275.25">
-      <c r="A10" s="71">
+      <c r="G9" s="77"/>
+    </row>
+    <row r="10" spans="1:28" s="67" customFormat="1" ht="121.5">
+      <c r="A10" s="68">
         <v>3</v>
       </c>
-      <c r="B10" s="104" t="s">
+      <c r="B10" s="76" t="s">
         <v>121</v>
       </c>
-      <c r="C10" s="104" t="s">
+      <c r="C10" s="76" t="s">
         <v>122</v>
       </c>
-      <c r="D10" s="104" t="s">
+      <c r="D10" s="76" t="s">
         <v>123</v>
       </c>
-      <c r="E10" s="104" t="s">
+      <c r="E10" s="76" t="s">
         <v>124</v>
       </c>
-      <c r="F10" s="104" t="s">
+      <c r="F10" s="76" t="s">
         <v>125</v>
       </c>
-      <c r="G10" s="104"/>
-      <c r="H10" s="67"/>
+      <c r="G10" s="76"/>
+      <c r="H10" s="66"/>
     </row>
     <row r="11" spans="1:28" s="61" customFormat="1" ht="60.75">
-      <c r="A11" s="72">
+      <c r="A11" s="69">
         <v>4</v>
       </c>
-      <c r="B11" s="106" t="s">
+      <c r="B11" s="78" t="s">
         <v>97</v>
       </c>
-      <c r="C11" s="106" t="s">
+      <c r="C11" s="78" t="s">
         <v>98</v>
       </c>
-      <c r="D11" s="106" t="s">
+      <c r="D11" s="78" t="s">
         <v>99</v>
       </c>
-      <c r="E11" s="106"/>
-      <c r="F11" s="106"/>
-      <c r="G11" s="106"/>
+      <c r="E11" s="78"/>
+      <c r="F11" s="78"/>
+      <c r="G11" s="78"/>
     </row>
     <row r="12" spans="1:28" s="61" customFormat="1" ht="76.5">
-      <c r="A12" s="71">
+      <c r="A12" s="68">
         <v>5</v>
       </c>
-      <c r="B12" s="104"/>
-      <c r="C12" s="104" t="s">
+      <c r="B12" s="76"/>
+      <c r="C12" s="76" t="s">
         <v>111</v>
       </c>
-      <c r="D12" s="104" t="s">
+      <c r="D12" s="76" t="s">
         <v>112</v>
       </c>
-      <c r="E12" s="104"/>
-      <c r="F12" s="104"/>
-      <c r="G12" s="104"/>
-    </row>
-    <row r="13" spans="1:28" s="55" customFormat="1" ht="244.5">
-      <c r="A13" s="72">
+      <c r="E12" s="76"/>
+      <c r="F12" s="76"/>
+      <c r="G12" s="76"/>
+    </row>
+    <row r="13" spans="1:28" s="55" customFormat="1" ht="198">
+      <c r="A13" s="69">
         <v>6</v>
       </c>
-      <c r="B13" s="73" t="s">
+      <c r="B13" s="70" t="s">
         <v>256</v>
       </c>
-      <c r="C13" s="106"/>
-      <c r="D13" s="106"/>
-      <c r="E13" s="73" t="s">
+      <c r="C13" s="78"/>
+      <c r="D13" s="78"/>
+      <c r="E13" s="70" t="s">
         <v>257</v>
       </c>
-      <c r="F13" s="73" t="s">
+      <c r="F13" s="70" t="s">
         <v>258</v>
       </c>
-      <c r="G13" s="106"/>
-    </row>
-    <row r="14" spans="1:28" s="55" customFormat="1" ht="167.25">
-      <c r="A14" s="71">
+      <c r="G13" s="78"/>
+    </row>
+    <row r="14" spans="1:28" s="55" customFormat="1" ht="152.25">
+      <c r="A14" s="68">
         <v>7</v>
       </c>
-      <c r="B14" s="74" t="s">
+      <c r="B14" s="71" t="s">
         <v>259</v>
       </c>
-      <c r="C14" s="104"/>
-      <c r="D14" s="104"/>
-      <c r="E14" s="74" t="s">
+      <c r="C14" s="76"/>
+      <c r="D14" s="76"/>
+      <c r="E14" s="71" t="s">
         <v>260</v>
       </c>
-      <c r="F14" s="74" t="s">
+      <c r="F14" s="71" t="s">
         <v>261</v>
       </c>
-      <c r="G14" s="104"/>
-    </row>
-    <row r="15" spans="1:28" s="55" customFormat="1" ht="244.5">
-      <c r="A15" s="72">
+      <c r="G14" s="76"/>
+    </row>
+    <row r="15" spans="1:28" s="55" customFormat="1" ht="213">
+      <c r="A15" s="69">
         <v>8</v>
       </c>
-      <c r="B15" s="73" t="s">
+      <c r="B15" s="70" t="s">
         <v>262</v>
       </c>
-      <c r="C15" s="106"/>
-      <c r="D15" s="106"/>
-      <c r="E15" s="73" t="s">
+      <c r="C15" s="78"/>
+      <c r="D15" s="78"/>
+      <c r="E15" s="70" t="s">
         <v>257</v>
       </c>
-      <c r="F15" s="73" t="s">
+      <c r="F15" s="70" t="s">
         <v>263</v>
       </c>
-      <c r="G15" s="106"/>
-    </row>
-    <row r="16" spans="1:28" s="55" customFormat="1" ht="183">
-      <c r="A16" s="71">
+      <c r="G15" s="78"/>
+    </row>
+    <row r="16" spans="1:28" s="55" customFormat="1" ht="167.25">
+      <c r="A16" s="68">
         <v>9</v>
       </c>
-      <c r="B16" s="74" t="s">
+      <c r="B16" s="71" t="s">
         <v>264</v>
       </c>
-      <c r="C16" s="104"/>
-      <c r="D16" s="104"/>
-      <c r="E16" s="74" t="s">
+      <c r="C16" s="76"/>
+      <c r="D16" s="76"/>
+      <c r="E16" s="71" t="s">
         <v>260</v>
       </c>
-      <c r="F16" s="74" t="s">
+      <c r="F16" s="71" t="s">
         <v>265</v>
       </c>
-      <c r="G16" s="104"/>
-    </row>
-    <row r="17" spans="1:7" s="55" customFormat="1" ht="183">
-      <c r="A17" s="72">
+      <c r="G16" s="76"/>
+    </row>
+    <row r="17" spans="1:7" s="55" customFormat="1" ht="167.25">
+      <c r="A17" s="69">
         <v>10</v>
       </c>
-      <c r="B17" s="73" t="s">
+      <c r="B17" s="70" t="s">
         <v>266</v>
       </c>
-      <c r="C17" s="106"/>
-      <c r="D17" s="106"/>
-      <c r="E17" s="73" t="s">
+      <c r="C17" s="78"/>
+      <c r="D17" s="78"/>
+      <c r="E17" s="70" t="s">
         <v>260</v>
       </c>
-      <c r="F17" s="73" t="s">
+      <c r="F17" s="70" t="s">
         <v>267</v>
       </c>
-      <c r="G17" s="106"/>
-    </row>
-    <row r="18" spans="1:7" s="55" customFormat="1" ht="167.25">
-      <c r="A18" s="71">
+      <c r="G17" s="78"/>
+    </row>
+    <row r="18" spans="1:7" s="55" customFormat="1" ht="137.25">
+      <c r="A18" s="68">
         <v>11</v>
       </c>
-      <c r="B18" s="74" t="s">
+      <c r="B18" s="71" t="s">
         <v>268</v>
       </c>
-      <c r="C18" s="104"/>
-      <c r="D18" s="104"/>
-      <c r="E18" s="74" t="s">
+      <c r="C18" s="76"/>
+      <c r="D18" s="76"/>
+      <c r="E18" s="71" t="s">
         <v>269</v>
       </c>
-      <c r="F18" s="74" t="s">
+      <c r="F18" s="71" t="s">
         <v>270</v>
       </c>
-      <c r="G18" s="104"/>
+      <c r="G18" s="76"/>
     </row>
     <row r="19" spans="1:7" s="55" customFormat="1" ht="102.75" customHeight="1">
-      <c r="A19" s="72">
+      <c r="A19" s="69">
         <v>12</v>
       </c>
-      <c r="B19" s="106" t="s">
+      <c r="B19" s="78" t="s">
         <v>271</v>
       </c>
-      <c r="C19" s="106"/>
-      <c r="D19" s="106"/>
-      <c r="E19" s="106"/>
-      <c r="F19" s="106" t="s">
+      <c r="C19" s="78"/>
+      <c r="D19" s="78"/>
+      <c r="E19" s="78"/>
+      <c r="F19" s="78" t="s">
         <v>272</v>
       </c>
-      <c r="G19" s="106"/>
-    </row>
-    <row r="20" spans="1:7" s="55" customFormat="1" ht="213">
-      <c r="A20" s="71">
+      <c r="G19" s="78"/>
+    </row>
+    <row r="20" spans="1:7" s="55" customFormat="1" ht="183">
+      <c r="A20" s="68">
         <v>13</v>
       </c>
-      <c r="B20" s="104" t="s">
+      <c r="B20" s="76" t="s">
         <v>273</v>
       </c>
-      <c r="C20" s="104"/>
-      <c r="D20" s="104"/>
-      <c r="E20" s="104"/>
-      <c r="F20" s="104" t="s">
+      <c r="C20" s="76"/>
+      <c r="D20" s="76"/>
+      <c r="E20" s="76"/>
+      <c r="F20" s="76" t="s">
         <v>274</v>
       </c>
-      <c r="G20" s="104"/>
+      <c r="G20" s="76"/>
     </row>
     <row r="21" spans="1:7" s="55" customFormat="1" ht="75" customHeight="1">
-      <c r="A21" s="75">
+      <c r="A21" s="69">
         <v>14</v>
       </c>
-      <c r="B21" s="107" t="s">
+      <c r="B21" s="78" t="s">
         <v>275</v>
       </c>
-      <c r="C21" s="107" t="s">
+      <c r="C21" s="78" t="s">
         <v>276</v>
       </c>
-      <c r="D21" s="107"/>
-      <c r="E21" s="107"/>
-      <c r="F21" s="107" t="s">
+      <c r="D21" s="78"/>
+      <c r="E21" s="78"/>
+      <c r="F21" s="78" t="s">
         <v>277</v>
       </c>
-      <c r="G21" s="107"/>
+      <c r="G21" s="78"/>
     </row>
     <row r="22" spans="1:7" s="55" customFormat="1" ht="180" customHeight="1">
-      <c r="A22" s="71">
+      <c r="A22" s="68">
         <v>15</v>
       </c>
-      <c r="B22" s="104" t="s">
+      <c r="B22" s="76" t="s">
         <v>278</v>
       </c>
-      <c r="C22" s="104"/>
-      <c r="D22" s="104"/>
-      <c r="E22" s="104" t="s">
+      <c r="C22" s="76"/>
+      <c r="D22" s="76"/>
+      <c r="E22" s="76" t="s">
         <v>279</v>
       </c>
-      <c r="F22" s="104" t="s">
+      <c r="F22" s="76" t="s">
         <v>280</v>
       </c>
-      <c r="G22" s="104" t="s">
+      <c r="G22" s="76" t="s">
         <v>281</v>
       </c>
     </row>
     <row r="23" spans="1:7" s="55" customFormat="1" ht="229.5">
-      <c r="A23" s="76">
+      <c r="A23" s="87">
         <v>16</v>
       </c>
-      <c r="B23" s="108" t="s">
+      <c r="B23" s="83" t="s">
         <v>282</v>
       </c>
-      <c r="C23" s="77" t="s">
+      <c r="C23" s="76" t="s">
         <v>283</v>
       </c>
-      <c r="D23" s="77" t="s">
+      <c r="D23" s="76" t="s">
         <v>284</v>
       </c>
-      <c r="E23" s="108" t="s">
+      <c r="E23" s="83" t="s">
         <v>285</v>
       </c>
-      <c r="F23" s="108" t="s">
+      <c r="F23" s="83" t="s">
         <v>286</v>
       </c>
-      <c r="G23" s="109"/>
+      <c r="G23" s="84"/>
     </row>
     <row r="24" spans="1:7" s="55" customFormat="1" ht="409.6">
-      <c r="A24" s="91">
+      <c r="A24" s="88">
         <v>17</v>
       </c>
-      <c r="B24" s="110" t="s">
+      <c r="B24" s="79" t="s">
         <v>287</v>
       </c>
-      <c r="C24" s="110" t="s">
+      <c r="C24" s="79" t="s">
         <v>288</v>
       </c>
-      <c r="D24" s="110" t="s">
+      <c r="D24" s="79" t="s">
         <v>289</v>
       </c>
-      <c r="E24" s="110" t="s">
+      <c r="E24" s="79" t="s">
         <v>290</v>
       </c>
-      <c r="F24" s="110" t="s">
+      <c r="F24" s="79" t="s">
         <v>291</v>
       </c>
-      <c r="G24" s="110"/>
+      <c r="G24" s="79"/>
     </row>
     <row r="25" spans="1:7" s="55" customFormat="1" ht="229.5">
-      <c r="A25" s="81">
+      <c r="A25" s="89">
         <v>18</v>
       </c>
-      <c r="B25" s="82" t="s">
+      <c r="B25" s="90" t="s">
         <v>292</v>
       </c>
-      <c r="C25" s="61" t="s">
+      <c r="C25" s="83" t="s">
         <v>293</v>
       </c>
-      <c r="D25" s="83" t="s">
+      <c r="D25" s="91" t="s">
         <v>294</v>
       </c>
-      <c r="E25" s="84" t="s">
+      <c r="E25" s="92" t="s">
         <v>295</v>
       </c>
-      <c r="F25" s="84" t="s">
+      <c r="F25" s="92" t="s">
         <v>296</v>
       </c>
-      <c r="G25" s="78"/>
+      <c r="G25" s="84"/>
     </row>
     <row r="26" spans="1:7" s="55" customFormat="1" ht="409.6">
-      <c r="A26" s="92">
+      <c r="A26" s="72">
         <v>19</v>
       </c>
-      <c r="B26" s="93" t="s">
+      <c r="B26" s="80" t="s">
         <v>297</v>
       </c>
-      <c r="C26" s="94" t="s">
+      <c r="C26" s="79" t="s">
         <v>298</v>
       </c>
-      <c r="D26" s="94" t="s">
+      <c r="D26" s="79" t="s">
         <v>299</v>
       </c>
-      <c r="E26" s="95" t="s">
+      <c r="E26" s="81" t="s">
         <v>300</v>
       </c>
-      <c r="F26" s="95" t="s">
+      <c r="F26" s="81" t="s">
         <v>301</v>
       </c>
-      <c r="G26" s="96"/>
+      <c r="G26" s="82"/>
     </row>
     <row r="27" spans="1:7" s="55" customFormat="1" ht="396.75">
-      <c r="A27" s="98">
+      <c r="A27" s="87">
         <v>20</v>
       </c>
-      <c r="B27" s="80" t="s">
+      <c r="B27" s="93" t="s">
         <v>302</v>
       </c>
-      <c r="C27" s="80" t="s">
+      <c r="C27" s="93" t="s">
         <v>303</v>
       </c>
-      <c r="D27" s="61" t="s">
+      <c r="D27" s="83" t="s">
         <v>304</v>
       </c>
-      <c r="E27" s="99" t="s">
+      <c r="E27" s="83" t="s">
         <v>305</v>
       </c>
-      <c r="F27" s="99" t="s">
+      <c r="F27" s="83" t="s">
         <v>306</v>
       </c>
-      <c r="G27" s="100"/>
+      <c r="G27" s="84"/>
     </row>
     <row r="28" spans="1:7" s="55" customFormat="1" ht="275.25">
-      <c r="A28" s="101">
+      <c r="A28" s="73">
         <v>21</v>
       </c>
-      <c r="B28" s="96" t="s">
+      <c r="B28" s="82" t="s">
         <v>307</v>
       </c>
-      <c r="C28" s="96" t="s">
+      <c r="C28" s="82" t="s">
         <v>307</v>
       </c>
-      <c r="D28" s="97" t="s">
+      <c r="D28" s="79" t="s">
         <v>308</v>
       </c>
-      <c r="E28" s="97" t="s">
+      <c r="E28" s="79" t="s">
         <v>309</v>
       </c>
-      <c r="F28" s="97" t="s">
+      <c r="F28" s="79" t="s">
         <v>310</v>
       </c>
-      <c r="G28" s="96"/>
+      <c r="G28" s="82"/>
     </row>
     <row r="29" spans="1:7" s="55" customFormat="1" ht="138" customHeight="1">
-      <c r="A29" s="102">
+      <c r="A29" s="74">
         <v>22</v>
       </c>
-      <c r="B29" s="66" t="s">
+      <c r="B29" s="83" t="s">
         <v>311</v>
       </c>
-      <c r="C29" s="66"/>
-      <c r="D29" s="66"/>
-      <c r="E29" s="66" t="s">
+      <c r="C29" s="84"/>
+      <c r="D29" s="84"/>
+      <c r="E29" s="84" t="s">
         <v>312</v>
       </c>
-      <c r="F29" s="79" t="s">
+      <c r="F29" s="83" t="s">
         <v>313</v>
       </c>
-      <c r="G29" s="79" t="s">
+      <c r="G29" s="83" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="30" spans="1:7" s="55" customFormat="1">
-      <c r="A30" s="66"/>
-      <c r="B30" s="66"/>
-      <c r="C30" s="66"/>
-      <c r="D30" s="66"/>
-      <c r="E30" s="66"/>
-      <c r="F30" s="66"/>
-      <c r="G30" s="66"/>
+    <row r="30" spans="1:7" s="55" customFormat="1" ht="351">
+      <c r="A30" s="73">
+        <v>23</v>
+      </c>
+      <c r="B30" s="79" t="s">
+        <v>315</v>
+      </c>
+      <c r="C30" s="79" t="s">
+        <v>316</v>
+      </c>
+      <c r="D30" s="79" t="s">
+        <v>317</v>
+      </c>
+      <c r="E30" s="79" t="s">
+        <v>318</v>
+      </c>
+      <c r="F30" s="79" t="s">
+        <v>319</v>
+      </c>
+      <c r="G30" s="82"/>
     </row>
     <row r="31" spans="1:7" s="55" customFormat="1"/>
     <row r="32" spans="1:7" s="55" customFormat="1"/>
@@ -65758,7 +65751,7 @@
         <v>119</v>
       </c>
       <c r="G2" s="28" t="s">
-        <v>315</v>
+        <v>320</v>
       </c>
       <c r="H2" s="25"/>
     </row>

</xml_diff>